<commit_message>
Updated picrust PCA and made barplot
</commit_message>
<xml_diff>
--- a/data/40_core-microbiome/core_indval_genus.xlsx
+++ b/data/40_core-microbiome/core_indval_genus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alma/Documents/ubc/MICB575/project-2/micb475-team9/data/40_core-microbiome/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3BB78151-B45F-B54D-81AD-C91B80FB7022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CA153C38-C51C-2042-B684-183A41CA8FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
   </bookViews>
@@ -1720,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>